<commit_message>
final commit before presentation
</commit_message>
<xml_diff>
--- a/iForm_Order3_SimulationResults.xlsx
+++ b/iForm_Order3_SimulationResults.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="20730" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Simulation1" sheetId="1" r:id="rId1"/>
     <sheet name="Simulation2" sheetId="2" r:id="rId2"/>
     <sheet name="Simulation3" sheetId="3" r:id="rId3"/>
     <sheet name="Simulation4" sheetId="4" r:id="rId4"/>
+    <sheet name="FuncSimulation" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="25">
   <si>
     <t>Model</t>
   </si>
@@ -86,6 +87,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Polynomial Degree</t>
+  </si>
+  <si>
+    <t>Model Predictors</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1142,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2896,4 +2903,73 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.14169999999999999</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>0.71250000000000002</v>
+      </c>
+      <c r="C3">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.9667</v>
+      </c>
+      <c r="E3">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>